<commit_message>
This files contain case studeis on linear programming binry programmin and no linear
</commit_message>
<xml_diff>
--- a/shipping_problem.xlsx
+++ b/shipping_problem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Downloads\Python\excel\bussiness_development_course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BC7DC1D-1702-4355-927B-3053744C158D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5C7C15-BA93-4A3E-A9E1-0729E90D980F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{02EAAC21-4280-4B36-A29C-92E61F17993A}"/>
   </bookViews>
@@ -218,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -239,21 +239,20 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -921,7 +920,7 @@
   <dimension ref="B9:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -959,19 +958,19 @@
       </c>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>10</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <v>4</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <v>9</v>
       </c>
       <c r="G11" s="3">
@@ -979,17 +978,17 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="13"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <v>12</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="10">
         <v>6</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <v>8</v>
       </c>
       <c r="G12" s="3">
@@ -997,17 +996,17 @@
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="13"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="10">
         <v>8</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="10">
         <v>9</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="10">
         <v>5</v>
       </c>
       <c r="G13" s="3">
@@ -1051,13 +1050,13 @@
       <c r="C19" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <v>40</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="8">
         <v>40</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="8">
         <v>0</v>
       </c>
       <c r="G19" s="7">
@@ -1069,13 +1068,13 @@
       <c r="C20" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <v>0</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <v>0</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="8">
         <v>40</v>
       </c>
       <c r="G20" s="7">
@@ -1087,17 +1086,17 @@
       <c r="C21" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="8">
         <v>10</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="8">
         <v>0</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="8">
         <v>20</v>
       </c>
       <c r="G21" s="7">
-        <f t="shared" ref="G20:G21" si="0">SUM(D21:F21)</f>
+        <f t="shared" ref="G21" si="0">SUM(D21:F21)</f>
         <v>30</v>
       </c>
     </row>
@@ -1117,10 +1116,10 @@
         <f>SUM(F19:F21)</f>
         <v>60</v>
       </c>
-      <c r="G22" s="8"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D25">

</xml_diff>